<commit_message>
upgrade version of extracting column from excel
</commit_message>
<xml_diff>
--- a/Projects/Vehicle Access Card/Reminder.xlsx
+++ b/Projects/Vehicle Access Card/Reminder.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,11 +440,6 @@
           <t>Access card no</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Vehicle no</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -458,11 +453,6 @@
       <c r="C2" t="n">
         <v>102</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>B22345</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -476,11 +466,6 @@
       <c r="C3" t="n">
         <v>103</v>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>C32345</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -494,11 +479,6 @@
       <c r="C4" t="n">
         <v>104</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>D42345</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -512,11 +492,6 @@
       <c r="C5" t="n">
         <v>105</v>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>E52345</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -530,11 +505,6 @@
       <c r="C6" t="n">
         <v>108</v>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>H82345</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -547,11 +517,6 @@
       </c>
       <c r="C7" t="n">
         <v>109</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>I92345</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>